<commit_message>
Merge between testing and master 2 for new update features  (#5)
* Check file extension and display information for user

* Update route and chart in index.js

* Add meeting minutes

* add a bulk upload in web interface and change a bit of different roles interface

* remove employees paid salaries
</commit_message>
<xml_diff>
--- a/Resources/UnitBudgetProjectArchive/CSSE Sem1, FICTICIOUS Unit budgets SUMMARY.xlsx
+++ b/Resources/UnitBudgetProjectArchive/CSSE Sem1, FICTICIOUS Unit budgets SUMMARY.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10808"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/00047104/Dropbox/CITS5206-MITcapstone-2021/projectsfor2021/CSSEunitbudgetsdatabase/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sameam/Desktop/OneDrive/Desktop/Professional/project1/Unit_Budget_Planner/Resources/UnitBudgetProjectArchive/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DE502F2-A83D-0B4A-B563-EE2CE1DE2C46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{381C403A-2621-8441-956B-1C9C80A7CF43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2920" yWindow="4580" windowWidth="28100" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="700" yWindow="500" windowWidth="28100" windowHeight="16400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1026,7 +1026,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1035,12 +1035,13 @@
     <col min="2" max="2" width="62.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.83203125" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" customWidth="1"/>
     <col min="6" max="6" width="12.5" customWidth="1"/>
     <col min="7" max="7" width="11.1640625" style="16" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.1640625" style="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="5" customFormat="1" ht="80" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="5" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>40</v>
       </c>

</xml_diff>